<commit_message>
search ip gui finish
</commit_message>
<xml_diff>
--- a/data/mypc_dummy.xlsx
+++ b/data/mypc_dummy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\IPC\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F772AA0-CD63-48D0-96F6-E7E565BE4E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="1128" windowWidth="17280" windowHeight="10728" activeTab="2"/>
+    <workbookView xWindow="1020" yWindow="708" windowWidth="17280" windowHeight="10728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,7 +383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView topLeftCell="A97" workbookViewId="0">
@@ -392,6 +393,7 @@
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
@@ -2096,7 +2098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2104,6 +2106,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -3807,14 +3812,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
student mypc page search finish
</commit_message>
<xml_diff>
--- a/data/mypc_dummy.xlsx
+++ b/data/mypc_dummy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F772AA0-CD63-48D0-96F6-E7E565BE4E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181CB9E0-D9D4-4B0F-BA67-768E94ACAE38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="708" windowWidth="17280" windowHeight="10728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="1692" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -415,7 +415,7 @@
         <v>1101</v>
       </c>
       <c r="B2">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -429,7 +429,7 @@
         <v>1102</v>
       </c>
       <c r="B3">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -443,7 +443,7 @@
         <v>1103</v>
       </c>
       <c r="B4">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -457,7 +457,7 @@
         <v>1104</v>
       </c>
       <c r="B5">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -471,7 +471,7 @@
         <v>1105</v>
       </c>
       <c r="B6">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -485,7 +485,7 @@
         <v>1106</v>
       </c>
       <c r="B7">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -499,7 +499,7 @@
         <v>1107</v>
       </c>
       <c r="B8">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -513,7 +513,7 @@
         <v>1108</v>
       </c>
       <c r="B9">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C9">
         <v>90</v>
@@ -527,7 +527,7 @@
         <v>1109</v>
       </c>
       <c r="B10">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -541,7 +541,7 @@
         <v>1110</v>
       </c>
       <c r="B11">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -555,7 +555,7 @@
         <v>1111</v>
       </c>
       <c r="B12">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -569,7 +569,7 @@
         <v>1112</v>
       </c>
       <c r="B13">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -583,7 +583,7 @@
         <v>1113</v>
       </c>
       <c r="B14">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -597,7 +597,7 @@
         <v>1114</v>
       </c>
       <c r="B15">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -611,7 +611,7 @@
         <v>1115</v>
       </c>
       <c r="B16">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -625,7 +625,7 @@
         <v>1116</v>
       </c>
       <c r="B17">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C17">
         <v>100</v>
@@ -639,7 +639,7 @@
         <v>1117</v>
       </c>
       <c r="B18">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -653,7 +653,7 @@
         <v>1118</v>
       </c>
       <c r="B19">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C19">
         <v>100</v>
@@ -667,7 +667,7 @@
         <v>1119</v>
       </c>
       <c r="B20">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -681,7 +681,7 @@
         <v>1120</v>
       </c>
       <c r="B21">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -695,7 +695,7 @@
         <v>1201</v>
       </c>
       <c r="B22">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -709,7 +709,7 @@
         <v>1202</v>
       </c>
       <c r="B23">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -723,7 +723,7 @@
         <v>1203</v>
       </c>
       <c r="B24">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C24">
         <v>90</v>
@@ -737,7 +737,7 @@
         <v>1204</v>
       </c>
       <c r="B25">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -751,7 +751,7 @@
         <v>1205</v>
       </c>
       <c r="B26">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C26">
         <v>100</v>
@@ -765,7 +765,7 @@
         <v>1206</v>
       </c>
       <c r="B27">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C27">
         <v>100</v>
@@ -779,7 +779,7 @@
         <v>1207</v>
       </c>
       <c r="B28">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C28">
         <v>100</v>
@@ -793,7 +793,7 @@
         <v>1208</v>
       </c>
       <c r="B29">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C29">
         <v>100</v>
@@ -807,7 +807,7 @@
         <v>1209</v>
       </c>
       <c r="B30">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C30">
         <v>100</v>
@@ -821,7 +821,7 @@
         <v>1210</v>
       </c>
       <c r="B31">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -835,7 +835,7 @@
         <v>1211</v>
       </c>
       <c r="B32">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -849,7 +849,7 @@
         <v>1212</v>
       </c>
       <c r="B33">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -863,7 +863,7 @@
         <v>1213</v>
       </c>
       <c r="B34">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -877,7 +877,7 @@
         <v>1214</v>
       </c>
       <c r="B35">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -891,7 +891,7 @@
         <v>1215</v>
       </c>
       <c r="B36">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C36">
         <v>100</v>
@@ -905,7 +905,7 @@
         <v>1216</v>
       </c>
       <c r="B37">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C37">
         <v>100</v>
@@ -919,7 +919,7 @@
         <v>1217</v>
       </c>
       <c r="B38">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C38">
         <v>90</v>
@@ -933,7 +933,7 @@
         <v>1218</v>
       </c>
       <c r="B39">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C39">
         <v>100</v>
@@ -947,7 +947,7 @@
         <v>1219</v>
       </c>
       <c r="B40">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -961,7 +961,7 @@
         <v>1220</v>
       </c>
       <c r="B41">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -975,7 +975,7 @@
         <v>1301</v>
       </c>
       <c r="B42">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C42">
         <v>100</v>
@@ -989,7 +989,7 @@
         <v>1302</v>
       </c>
       <c r="B43">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C43">
         <v>100</v>
@@ -1003,7 +1003,7 @@
         <v>1303</v>
       </c>
       <c r="B44">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -1017,7 +1017,7 @@
         <v>1304</v>
       </c>
       <c r="B45">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1031,7 +1031,7 @@
         <v>1305</v>
       </c>
       <c r="B46">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C46">
         <v>100</v>
@@ -1045,7 +1045,7 @@
         <v>1306</v>
       </c>
       <c r="B47">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C47">
         <v>100</v>
@@ -1059,7 +1059,7 @@
         <v>1307</v>
       </c>
       <c r="B48">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C48">
         <v>100</v>
@@ -1073,7 +1073,7 @@
         <v>1308</v>
       </c>
       <c r="B49">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C49">
         <v>100</v>
@@ -1087,7 +1087,7 @@
         <v>1309</v>
       </c>
       <c r="B50">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C50">
         <v>100</v>
@@ -1101,7 +1101,7 @@
         <v>1310</v>
       </c>
       <c r="B51">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C51">
         <v>100</v>
@@ -1115,7 +1115,7 @@
         <v>1311</v>
       </c>
       <c r="B52">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C52">
         <v>100</v>
@@ -1129,7 +1129,7 @@
         <v>1312</v>
       </c>
       <c r="B53">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C53">
         <v>90</v>
@@ -1143,7 +1143,7 @@
         <v>1313</v>
       </c>
       <c r="B54">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C54">
         <v>100</v>
@@ -1157,7 +1157,7 @@
         <v>1314</v>
       </c>
       <c r="B55">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C55">
         <v>100</v>
@@ -1171,7 +1171,7 @@
         <v>1315</v>
       </c>
       <c r="B56">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C56">
         <v>100</v>
@@ -1185,7 +1185,7 @@
         <v>1316</v>
       </c>
       <c r="B57">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C57">
         <v>100</v>
@@ -1199,7 +1199,7 @@
         <v>1317</v>
       </c>
       <c r="B58">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C58">
         <v>100</v>
@@ -1213,7 +1213,7 @@
         <v>1318</v>
       </c>
       <c r="B59">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C59">
         <v>100</v>
@@ -1227,7 +1227,7 @@
         <v>1319</v>
       </c>
       <c r="B60">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C60">
         <v>100</v>
@@ -1241,7 +1241,7 @@
         <v>1320</v>
       </c>
       <c r="B61">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C61">
         <v>100</v>
@@ -1255,7 +1255,7 @@
         <v>1401</v>
       </c>
       <c r="B62">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C62">
         <v>100</v>
@@ -1269,7 +1269,7 @@
         <v>1402</v>
       </c>
       <c r="B63">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C63">
         <v>100</v>
@@ -1283,7 +1283,7 @@
         <v>1403</v>
       </c>
       <c r="B64">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C64">
         <v>100</v>
@@ -1297,7 +1297,7 @@
         <v>1404</v>
       </c>
       <c r="B65">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C65">
         <v>90</v>
@@ -1311,7 +1311,7 @@
         <v>1405</v>
       </c>
       <c r="B66">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C66">
         <v>100</v>
@@ -1325,7 +1325,7 @@
         <v>1406</v>
       </c>
       <c r="B67">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C67">
         <v>100</v>
@@ -1339,7 +1339,7 @@
         <v>1407</v>
       </c>
       <c r="B68">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C68">
         <v>90</v>
@@ -1353,7 +1353,7 @@
         <v>1408</v>
       </c>
       <c r="B69">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C69">
         <v>100</v>
@@ -1367,7 +1367,7 @@
         <v>1409</v>
       </c>
       <c r="B70">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C70">
         <v>100</v>
@@ -1381,7 +1381,7 @@
         <v>1410</v>
       </c>
       <c r="B71">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C71">
         <v>100</v>
@@ -1395,7 +1395,7 @@
         <v>1411</v>
       </c>
       <c r="B72">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C72">
         <v>100</v>
@@ -1409,7 +1409,7 @@
         <v>1412</v>
       </c>
       <c r="B73">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C73">
         <v>100</v>
@@ -1423,7 +1423,7 @@
         <v>1413</v>
       </c>
       <c r="B74">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C74">
         <v>100</v>
@@ -1437,7 +1437,7 @@
         <v>1414</v>
       </c>
       <c r="B75">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C75">
         <v>100</v>
@@ -1451,7 +1451,7 @@
         <v>1415</v>
       </c>
       <c r="B76">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C76">
         <v>100</v>
@@ -1465,7 +1465,7 @@
         <v>1416</v>
       </c>
       <c r="B77">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C77">
         <v>100</v>
@@ -1479,7 +1479,7 @@
         <v>1417</v>
       </c>
       <c r="B78">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C78">
         <v>100</v>
@@ -1493,7 +1493,7 @@
         <v>1418</v>
       </c>
       <c r="B79">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C79">
         <v>100</v>
@@ -1507,7 +1507,7 @@
         <v>1419</v>
       </c>
       <c r="B80">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C80">
         <v>100</v>
@@ -1521,7 +1521,7 @@
         <v>1420</v>
       </c>
       <c r="B81">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C81">
         <v>100</v>
@@ -1535,7 +1535,7 @@
         <v>1501</v>
       </c>
       <c r="B82">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C82">
         <v>100</v>
@@ -1549,7 +1549,7 @@
         <v>1502</v>
       </c>
       <c r="B83">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C83">
         <v>100</v>
@@ -1563,7 +1563,7 @@
         <v>1503</v>
       </c>
       <c r="B84">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C84">
         <v>100</v>
@@ -1577,7 +1577,7 @@
         <v>1504</v>
       </c>
       <c r="B85">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C85">
         <v>100</v>
@@ -1591,7 +1591,7 @@
         <v>1505</v>
       </c>
       <c r="B86">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C86">
         <v>100</v>
@@ -1605,7 +1605,7 @@
         <v>1506</v>
       </c>
       <c r="B87">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C87">
         <v>100</v>
@@ -1619,7 +1619,7 @@
         <v>1507</v>
       </c>
       <c r="B88">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C88">
         <v>100</v>
@@ -1633,7 +1633,7 @@
         <v>1508</v>
       </c>
       <c r="B89">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C89">
         <v>100</v>
@@ -1647,7 +1647,7 @@
         <v>1509</v>
       </c>
       <c r="B90">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C90">
         <v>100</v>
@@ -1661,7 +1661,7 @@
         <v>1510</v>
       </c>
       <c r="B91">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C91">
         <v>100</v>
@@ -1675,7 +1675,7 @@
         <v>1511</v>
       </c>
       <c r="B92">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C92">
         <v>100</v>
@@ -1689,7 +1689,7 @@
         <v>1512</v>
       </c>
       <c r="B93">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C93">
         <v>100</v>
@@ -1703,7 +1703,7 @@
         <v>1513</v>
       </c>
       <c r="B94">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C94">
         <v>100</v>
@@ -1717,7 +1717,7 @@
         <v>1514</v>
       </c>
       <c r="B95">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C95">
         <v>100</v>
@@ -1731,7 +1731,7 @@
         <v>1515</v>
       </c>
       <c r="B96">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C96">
         <v>100</v>
@@ -1745,7 +1745,7 @@
         <v>1516</v>
       </c>
       <c r="B97">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C97">
         <v>100</v>
@@ -1759,7 +1759,7 @@
         <v>1517</v>
       </c>
       <c r="B98">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C98">
         <v>90</v>
@@ -1773,7 +1773,7 @@
         <v>1518</v>
       </c>
       <c r="B99">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -1787,7 +1787,7 @@
         <v>1519</v>
       </c>
       <c r="B100">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C100">
         <v>100</v>
@@ -1801,7 +1801,7 @@
         <v>1520</v>
       </c>
       <c r="B101">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1815,7 +1815,7 @@
         <v>1601</v>
       </c>
       <c r="B102">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C102">
         <v>100</v>
@@ -1829,7 +1829,7 @@
         <v>1602</v>
       </c>
       <c r="B103">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C103">
         <v>100</v>
@@ -1843,7 +1843,7 @@
         <v>1603</v>
       </c>
       <c r="B104">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C104">
         <v>100</v>
@@ -1857,7 +1857,7 @@
         <v>1604</v>
       </c>
       <c r="B105">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C105">
         <v>100</v>
@@ -1871,7 +1871,7 @@
         <v>1605</v>
       </c>
       <c r="B106">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C106">
         <v>100</v>
@@ -1885,7 +1885,7 @@
         <v>1606</v>
       </c>
       <c r="B107">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C107">
         <v>100</v>
@@ -1899,7 +1899,7 @@
         <v>1607</v>
       </c>
       <c r="B108">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C108">
         <v>100</v>
@@ -1913,7 +1913,7 @@
         <v>1608</v>
       </c>
       <c r="B109">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C109">
         <v>100</v>
@@ -1927,7 +1927,7 @@
         <v>1609</v>
       </c>
       <c r="B110">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C110">
         <v>100</v>
@@ -1941,7 +1941,7 @@
         <v>1610</v>
       </c>
       <c r="B111">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C111">
         <v>100</v>
@@ -1955,7 +1955,7 @@
         <v>1611</v>
       </c>
       <c r="B112">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C112">
         <v>100</v>
@@ -1969,7 +1969,7 @@
         <v>1612</v>
       </c>
       <c r="B113">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C113">
         <v>100</v>
@@ -1983,7 +1983,7 @@
         <v>1613</v>
       </c>
       <c r="B114">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C114">
         <v>100</v>
@@ -1997,7 +1997,7 @@
         <v>1614</v>
       </c>
       <c r="B115">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C115">
         <v>100</v>
@@ -2011,7 +2011,7 @@
         <v>1615</v>
       </c>
       <c r="B116">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C116">
         <v>100</v>
@@ -2025,7 +2025,7 @@
         <v>1616</v>
       </c>
       <c r="B117">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C117">
         <v>100</v>
@@ -2039,7 +2039,7 @@
         <v>1617</v>
       </c>
       <c r="B118">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C118">
         <v>100</v>
@@ -2053,7 +2053,7 @@
         <v>1618</v>
       </c>
       <c r="B119">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C119">
         <v>100</v>
@@ -2067,7 +2067,7 @@
         <v>1619</v>
       </c>
       <c r="B120">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C120">
         <v>90</v>
@@ -2081,7 +2081,7 @@
         <v>1620</v>
       </c>
       <c r="B121">
-        <v>11.11</v>
+        <v>2020.11</v>
       </c>
       <c r="C121">
         <v>100</v>
@@ -3815,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5521,5 +5521,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
model directory add and db_connect class add
</commit_message>
<xml_diff>
--- a/data/mypc_dummy.xlsx
+++ b/data/mypc_dummy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\IPC\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4032B5A-1163-4B6F-978A-47C209188DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="708" windowWidth="17280" windowHeight="10728"/>
+    <workbookView xWindow="1812" yWindow="1056" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,11 +398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -429,7 +430,7 @@
         <v>1101</v>
       </c>
       <c r="B2" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -443,7 +444,7 @@
         <v>1102</v>
       </c>
       <c r="B3" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -2112,7 +2113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3826,7 +3827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
did not start mypc cal success & modify mypc_dummy
</commit_message>
<xml_diff>
--- a/data/mypc_dummy.xlsx
+++ b/data/mypc_dummy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IPC\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\IPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17BE8C7-AB23-44ED-9702-F77FF2B599C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="816" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="816" windowWidth="17280" windowHeight="10728"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="5">
   <si>
     <t>hakbun</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,31 +45,11 @@
     <t>empty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>한글 업데이트 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mac</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020-12-02  13:11:00 PM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020-12-02  18:11:00 PM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020-12-02  19:11:00 PM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,12 +67,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,11 +107,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -396,16 +405,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D245" sqref="D245"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.69921875" customWidth="1"/>
     <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -428,7 +437,7 @@
         <v>1101</v>
       </c>
       <c r="B2" s="1">
-        <v>44182.375</v>
+        <v>44182.5</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -441,8 +450,8 @@
       <c r="A3">
         <v>1102</v>
       </c>
-      <c r="B3" s="1">
-        <v>44182.375</v>
+      <c r="B3" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -456,7 +465,7 @@
         <v>1103</v>
       </c>
       <c r="B4" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -469,8 +478,8 @@
       <c r="A5">
         <v>1104</v>
       </c>
-      <c r="B5" s="1">
-        <v>44167.508333333331</v>
+      <c r="B5" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -483,8 +492,8 @@
       <c r="A6">
         <v>1105</v>
       </c>
-      <c r="B6" s="1">
-        <v>44167.507638888892</v>
+      <c r="B6" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -498,7 +507,7 @@
         <v>1106</v>
       </c>
       <c r="B7" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -512,7 +521,7 @@
         <v>1107</v>
       </c>
       <c r="B8" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -526,13 +535,13 @@
         <v>1108</v>
       </c>
       <c r="B9" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C9">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -540,7 +549,7 @@
         <v>1109</v>
       </c>
       <c r="B10" s="1">
-        <v>44167.511111111111</v>
+        <v>44182.625</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -554,7 +563,7 @@
         <v>1110</v>
       </c>
       <c r="B11" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -568,7 +577,7 @@
         <v>1111</v>
       </c>
       <c r="B12" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -582,7 +591,7 @@
         <v>1112</v>
       </c>
       <c r="B13" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -596,7 +605,7 @@
         <v>1113</v>
       </c>
       <c r="B14" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -610,7 +619,7 @@
         <v>1114</v>
       </c>
       <c r="B15" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -624,7 +633,7 @@
         <v>1115</v>
       </c>
       <c r="B16" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -638,7 +647,7 @@
         <v>1116</v>
       </c>
       <c r="B17" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C17">
         <v>100</v>
@@ -651,8 +660,8 @@
       <c r="A18">
         <v>1117</v>
       </c>
-      <c r="B18" s="1">
-        <v>44167.507638888892</v>
+      <c r="B18" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -666,7 +675,7 @@
         <v>1118</v>
       </c>
       <c r="B19" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C19">
         <v>100</v>
@@ -680,7 +689,7 @@
         <v>1119</v>
       </c>
       <c r="B20" s="1">
-        <v>44167.51458333333</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -694,7 +703,7 @@
         <v>1120</v>
       </c>
       <c r="B21" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -707,8 +716,8 @@
       <c r="A22">
         <v>1201</v>
       </c>
-      <c r="B22" s="1">
-        <v>44167.507638888892</v>
+      <c r="B22" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -722,7 +731,7 @@
         <v>1202</v>
       </c>
       <c r="B23" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -736,13 +745,13 @@
         <v>1203</v>
       </c>
       <c r="B24" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C24">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
@@ -750,7 +759,7 @@
         <v>1204</v>
       </c>
       <c r="B25" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -764,7 +773,7 @@
         <v>1205</v>
       </c>
       <c r="B26" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C26">
         <v>100</v>
@@ -778,7 +787,7 @@
         <v>1206</v>
       </c>
       <c r="B27" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C27">
         <v>100</v>
@@ -791,8 +800,8 @@
       <c r="A28">
         <v>1207</v>
       </c>
-      <c r="B28" s="1">
-        <v>44167.510416666664</v>
+      <c r="B28" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C28">
         <v>100</v>
@@ -806,7 +815,7 @@
         <v>1208</v>
       </c>
       <c r="B29" s="1">
-        <v>44167.535416666666</v>
+        <v>44182.375</v>
       </c>
       <c r="C29">
         <v>100</v>
@@ -820,7 +829,7 @@
         <v>1209</v>
       </c>
       <c r="B30" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C30">
         <v>100</v>
@@ -834,7 +843,7 @@
         <v>1210</v>
       </c>
       <c r="B31" s="1">
-        <v>44167.511111111111</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -848,7 +857,7 @@
         <v>1211</v>
       </c>
       <c r="B32" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -862,7 +871,7 @@
         <v>1212</v>
       </c>
       <c r="B33" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -875,8 +884,8 @@
       <c r="A34">
         <v>1213</v>
       </c>
-      <c r="B34" s="1">
-        <v>44167.507638888892</v>
+      <c r="B34" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -890,7 +899,7 @@
         <v>1214</v>
       </c>
       <c r="B35" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -904,7 +913,7 @@
         <v>1215</v>
       </c>
       <c r="B36" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C36">
         <v>100</v>
@@ -918,7 +927,7 @@
         <v>1216</v>
       </c>
       <c r="B37" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C37">
         <v>100</v>
@@ -932,13 +941,13 @@
         <v>1217</v>
       </c>
       <c r="B38" s="1">
-        <v>44167.509027777778</v>
+        <v>44182.375</v>
       </c>
       <c r="C38">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
@@ -946,7 +955,7 @@
         <v>1218</v>
       </c>
       <c r="B39" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C39">
         <v>100</v>
@@ -960,7 +969,7 @@
         <v>1219</v>
       </c>
       <c r="B40" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -974,7 +983,7 @@
         <v>1220</v>
       </c>
       <c r="B41" s="1">
-        <v>44167.521527777775</v>
+        <v>44182.5</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -988,7 +997,7 @@
         <v>1301</v>
       </c>
       <c r="B42" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C42">
         <v>100</v>
@@ -1002,7 +1011,7 @@
         <v>1302</v>
       </c>
       <c r="B43" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C43">
         <v>100</v>
@@ -1016,7 +1025,7 @@
         <v>1303</v>
       </c>
       <c r="B44" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -1030,7 +1039,7 @@
         <v>1304</v>
       </c>
       <c r="B45" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1044,7 +1053,7 @@
         <v>1305</v>
       </c>
       <c r="B46" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C46">
         <v>100</v>
@@ -1058,7 +1067,7 @@
         <v>1306</v>
       </c>
       <c r="B47" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C47">
         <v>100</v>
@@ -1072,7 +1081,7 @@
         <v>1307</v>
       </c>
       <c r="B48" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C48">
         <v>100</v>
@@ -1086,7 +1095,7 @@
         <v>1308</v>
       </c>
       <c r="B49" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C49">
         <v>100</v>
@@ -1100,7 +1109,7 @@
         <v>1309</v>
       </c>
       <c r="B50" s="1">
-        <v>44167.52847222222</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C50">
         <v>100</v>
@@ -1114,7 +1123,7 @@
         <v>1310</v>
       </c>
       <c r="B51" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C51">
         <v>100</v>
@@ -1127,8 +1136,8 @@
       <c r="A52">
         <v>1311</v>
       </c>
-      <c r="B52" s="1">
-        <v>44167.507638888892</v>
+      <c r="B52" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C52">
         <v>100</v>
@@ -1142,13 +1151,13 @@
         <v>1312</v>
       </c>
       <c r="B53" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C53">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
@@ -1156,7 +1165,7 @@
         <v>1313</v>
       </c>
       <c r="B54" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C54">
         <v>100</v>
@@ -1170,7 +1179,7 @@
         <v>1314</v>
       </c>
       <c r="B55" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C55">
         <v>100</v>
@@ -1184,7 +1193,7 @@
         <v>1315</v>
       </c>
       <c r="B56" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C56">
         <v>100</v>
@@ -1197,8 +1206,8 @@
       <c r="A57">
         <v>1316</v>
       </c>
-      <c r="B57" s="1">
-        <v>44167.507638888892</v>
+      <c r="B57" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C57">
         <v>100</v>
@@ -1212,7 +1221,7 @@
         <v>1317</v>
       </c>
       <c r="B58" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C58">
         <v>100</v>
@@ -1226,7 +1235,7 @@
         <v>1318</v>
       </c>
       <c r="B59" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C59">
         <v>100</v>
@@ -1240,7 +1249,7 @@
         <v>1319</v>
       </c>
       <c r="B60" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C60">
         <v>100</v>
@@ -1254,7 +1263,7 @@
         <v>1320</v>
       </c>
       <c r="B61" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C61">
         <v>100</v>
@@ -1268,7 +1277,7 @@
         <v>1401</v>
       </c>
       <c r="B62" s="1">
-        <v>44167.535416666666</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C62">
         <v>100</v>
@@ -1282,7 +1291,7 @@
         <v>1402</v>
       </c>
       <c r="B63" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C63">
         <v>100</v>
@@ -1295,8 +1304,8 @@
       <c r="A64">
         <v>1403</v>
       </c>
-      <c r="B64" s="1">
-        <v>44167.511111111111</v>
+      <c r="B64" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C64">
         <v>100</v>
@@ -1310,13 +1319,13 @@
         <v>1404</v>
       </c>
       <c r="B65" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C65">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
@@ -1324,7 +1333,7 @@
         <v>1405</v>
       </c>
       <c r="B66" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C66">
         <v>100</v>
@@ -1338,7 +1347,7 @@
         <v>1406</v>
       </c>
       <c r="B67" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C67">
         <v>100</v>
@@ -1352,13 +1361,13 @@
         <v>1407</v>
       </c>
       <c r="B68" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C68">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.4">
@@ -1366,7 +1375,7 @@
         <v>1408</v>
       </c>
       <c r="B69" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C69">
         <v>100</v>
@@ -1379,8 +1388,8 @@
       <c r="A70">
         <v>1409</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>9</v>
+      <c r="B70" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C70">
         <v>100</v>
@@ -1393,8 +1402,8 @@
       <c r="A71">
         <v>1410</v>
       </c>
-      <c r="B71" s="1">
-        <v>44167.507638888892</v>
+      <c r="B71" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C71">
         <v>100</v>
@@ -1408,7 +1417,7 @@
         <v>1411</v>
       </c>
       <c r="B72" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C72">
         <v>100</v>
@@ -1421,8 +1430,8 @@
       <c r="A73">
         <v>1412</v>
       </c>
-      <c r="B73" s="1">
-        <v>44167.507638888892</v>
+      <c r="B73" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C73">
         <v>100</v>
@@ -1436,7 +1445,7 @@
         <v>1413</v>
       </c>
       <c r="B74" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C74">
         <v>100</v>
@@ -1449,8 +1458,8 @@
       <c r="A75">
         <v>1414</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>8</v>
+      <c r="B75" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C75">
         <v>100</v>
@@ -1464,7 +1473,7 @@
         <v>1415</v>
       </c>
       <c r="B76" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C76">
         <v>100</v>
@@ -1478,7 +1487,7 @@
         <v>1416</v>
       </c>
       <c r="B77" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C77">
         <v>100</v>
@@ -1491,8 +1500,8 @@
       <c r="A78">
         <v>1417</v>
       </c>
-      <c r="B78" s="1">
-        <v>44167.507638888892</v>
+      <c r="B78" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C78">
         <v>100</v>
@@ -1506,7 +1515,7 @@
         <v>1418</v>
       </c>
       <c r="B79" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C79">
         <v>100</v>
@@ -1519,8 +1528,8 @@
       <c r="A80">
         <v>1419</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>7</v>
+      <c r="B80" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C80">
         <v>100</v>
@@ -1534,7 +1543,7 @@
         <v>1420</v>
       </c>
       <c r="B81" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C81">
         <v>100</v>
@@ -1548,7 +1557,7 @@
         <v>1501</v>
       </c>
       <c r="B82" s="1">
-        <v>44167.521527777775</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C82">
         <v>100</v>
@@ -1562,7 +1571,7 @@
         <v>1502</v>
       </c>
       <c r="B83" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C83">
         <v>100</v>
@@ -1576,7 +1585,7 @@
         <v>1503</v>
       </c>
       <c r="B84" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C84">
         <v>100</v>
@@ -1590,7 +1599,7 @@
         <v>1504</v>
       </c>
       <c r="B85" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C85">
         <v>100</v>
@@ -1604,7 +1613,7 @@
         <v>1505</v>
       </c>
       <c r="B86" s="1">
-        <v>44167.535416666666</v>
+        <v>44182.375</v>
       </c>
       <c r="C86">
         <v>100</v>
@@ -1617,8 +1626,8 @@
       <c r="A87">
         <v>1506</v>
       </c>
-      <c r="B87" s="1">
-        <v>44167.507638888892</v>
+      <c r="B87" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C87">
         <v>100</v>
@@ -1632,7 +1641,7 @@
         <v>1507</v>
       </c>
       <c r="B88" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C88">
         <v>100</v>
@@ -1646,7 +1655,7 @@
         <v>1508</v>
       </c>
       <c r="B89" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C89">
         <v>100</v>
@@ -1660,7 +1669,7 @@
         <v>1509</v>
       </c>
       <c r="B90" s="1">
-        <v>44167.513194444444</v>
+        <v>44182.5</v>
       </c>
       <c r="C90">
         <v>100</v>
@@ -1674,7 +1683,7 @@
         <v>1510</v>
       </c>
       <c r="B91" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C91">
         <v>100</v>
@@ -1688,7 +1697,7 @@
         <v>1511</v>
       </c>
       <c r="B92" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C92">
         <v>100</v>
@@ -1702,7 +1711,7 @@
         <v>1512</v>
       </c>
       <c r="B93" s="1">
-        <v>44167.521527777775</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C93">
         <v>100</v>
@@ -1716,7 +1725,7 @@
         <v>1513</v>
       </c>
       <c r="B94" s="1">
-        <v>44167.52847222222</v>
+        <v>44182.375</v>
       </c>
       <c r="C94">
         <v>100</v>
@@ -1729,8 +1738,8 @@
       <c r="A95">
         <v>1514</v>
       </c>
-      <c r="B95" s="1">
-        <v>44167.507638888892</v>
+      <c r="B95" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C95">
         <v>100</v>
@@ -1744,7 +1753,7 @@
         <v>1515</v>
       </c>
       <c r="B96" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.458333333336</v>
       </c>
       <c r="C96">
         <v>100</v>
@@ -1758,7 +1767,7 @@
         <v>1516</v>
       </c>
       <c r="B97" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C97">
         <v>100</v>
@@ -1772,13 +1781,13 @@
         <v>1517</v>
       </c>
       <c r="B98" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C98">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.4">
@@ -1786,7 +1795,7 @@
         <v>1518</v>
       </c>
       <c r="B99" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.458333333336</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -1800,7 +1809,7 @@
         <v>1519</v>
       </c>
       <c r="B100" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C100">
         <v>100</v>
@@ -1814,7 +1823,7 @@
         <v>1520</v>
       </c>
       <c r="B101" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -1828,7 +1837,7 @@
         <v>1601</v>
       </c>
       <c r="B102" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C102">
         <v>100</v>
@@ -1842,7 +1851,7 @@
         <v>1602</v>
       </c>
       <c r="B103" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.458333333336</v>
       </c>
       <c r="C103">
         <v>100</v>
@@ -1856,7 +1865,7 @@
         <v>1603</v>
       </c>
       <c r="B104" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C104">
         <v>100</v>
@@ -1870,7 +1879,7 @@
         <v>1604</v>
       </c>
       <c r="B105" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C105">
         <v>100</v>
@@ -1884,7 +1893,7 @@
         <v>1605</v>
       </c>
       <c r="B106" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C106">
         <v>100</v>
@@ -1898,7 +1907,7 @@
         <v>1606</v>
       </c>
       <c r="B107" s="1">
-        <v>44167.51458333333</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C107">
         <v>100</v>
@@ -1912,7 +1921,7 @@
         <v>1607</v>
       </c>
       <c r="B108" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.625</v>
       </c>
       <c r="C108">
         <v>100</v>
@@ -1925,8 +1934,8 @@
       <c r="A109">
         <v>1608</v>
       </c>
-      <c r="B109" s="1">
-        <v>44167.507638888892</v>
+      <c r="B109" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C109">
         <v>100</v>
@@ -1940,7 +1949,7 @@
         <v>1609</v>
       </c>
       <c r="B110" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C110">
         <v>100</v>
@@ -1954,7 +1963,7 @@
         <v>1610</v>
       </c>
       <c r="B111" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C111">
         <v>100</v>
@@ -1968,7 +1977,7 @@
         <v>1611</v>
       </c>
       <c r="B112" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C112">
         <v>100</v>
@@ -1981,8 +1990,8 @@
       <c r="A113">
         <v>1612</v>
       </c>
-      <c r="B113" s="1">
-        <v>44167.509027777778</v>
+      <c r="B113" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C113">
         <v>100</v>
@@ -1996,7 +2005,7 @@
         <v>1613</v>
       </c>
       <c r="B114" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C114">
         <v>100</v>
@@ -2010,7 +2019,7 @@
         <v>1614</v>
       </c>
       <c r="B115" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.5</v>
       </c>
       <c r="C115">
         <v>100</v>
@@ -2023,8 +2032,8 @@
       <c r="A116">
         <v>1615</v>
       </c>
-      <c r="B116" s="1">
-        <v>44167.512499999997</v>
+      <c r="B116" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C116">
         <v>100</v>
@@ -2038,7 +2047,7 @@
         <v>1616</v>
       </c>
       <c r="B117" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C117">
         <v>100</v>
@@ -2052,7 +2061,7 @@
         <v>1617</v>
       </c>
       <c r="B118" s="1">
-        <v>44167.510416666664</v>
+        <v>44182.375</v>
       </c>
       <c r="C118">
         <v>100</v>
@@ -2065,8 +2074,8 @@
       <c r="A119">
         <v>1618</v>
       </c>
-      <c r="B119" s="1">
-        <v>44167.507638888892</v>
+      <c r="B119" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C119">
         <v>100</v>
@@ -2080,13 +2089,13 @@
         <v>1619</v>
       </c>
       <c r="B120" s="1">
-        <v>44167.507638888892</v>
+        <v>44182.375</v>
       </c>
       <c r="C120">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.4">
@@ -2094,7 +2103,7 @@
         <v>1620</v>
       </c>
       <c r="B121" s="1">
-        <v>44167.511111111111</v>
+        <v>44182.666666666664</v>
       </c>
       <c r="C121">
         <v>100</v>
@@ -2107,8 +2116,8 @@
       <c r="A122">
         <v>2101</v>
       </c>
-      <c r="B122">
-        <v>11.11</v>
+      <c r="B122" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C122">
         <v>100</v>
@@ -2121,8 +2130,8 @@
       <c r="A123">
         <v>2102</v>
       </c>
-      <c r="B123">
-        <v>11.11</v>
+      <c r="B123" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C123">
         <v>100</v>
@@ -2135,8 +2144,8 @@
       <c r="A124">
         <v>2103</v>
       </c>
-      <c r="B124">
-        <v>11.11</v>
+      <c r="B124" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C124">
         <v>100</v>
@@ -2149,8 +2158,8 @@
       <c r="A125">
         <v>2104</v>
       </c>
-      <c r="B125">
-        <v>11.11</v>
+      <c r="B125" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C125">
         <v>100</v>
@@ -2160,16 +2169,16 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A126">
+      <c r="A126" s="2">
         <v>2105</v>
       </c>
-      <c r="B126">
-        <v>11.11</v>
-      </c>
-      <c r="C126">
+      <c r="B126" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C126" s="2">
         <v>-1</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2177,8 +2186,8 @@
       <c r="A127">
         <v>2106</v>
       </c>
-      <c r="B127">
-        <v>11.11</v>
+      <c r="B127" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C127">
         <v>100</v>
@@ -2191,8 +2200,8 @@
       <c r="A128">
         <v>2107</v>
       </c>
-      <c r="B128">
-        <v>11.11</v>
+      <c r="B128" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C128">
         <v>100</v>
@@ -2205,8 +2214,8 @@
       <c r="A129">
         <v>2108</v>
       </c>
-      <c r="B129">
-        <v>11.11</v>
+      <c r="B129" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C129">
         <v>100</v>
@@ -2219,22 +2228,22 @@
       <c r="A130">
         <v>2109</v>
       </c>
-      <c r="B130">
-        <v>11.11</v>
+      <c r="B130" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C130">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D130" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>2110</v>
       </c>
-      <c r="B131">
-        <v>11.11</v>
+      <c r="B131" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C131">
         <v>100</v>
@@ -2247,8 +2256,8 @@
       <c r="A132">
         <v>2111</v>
       </c>
-      <c r="B132">
-        <v>11.11</v>
+      <c r="B132" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C132">
         <v>100</v>
@@ -2261,22 +2270,22 @@
       <c r="A133">
         <v>2112</v>
       </c>
-      <c r="B133">
-        <v>11.11</v>
+      <c r="B133" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C133">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D133" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>2113</v>
       </c>
-      <c r="B134">
-        <v>11.11</v>
+      <c r="B134" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C134">
         <v>100</v>
@@ -2289,8 +2298,8 @@
       <c r="A135">
         <v>2114</v>
       </c>
-      <c r="B135">
-        <v>11.11</v>
+      <c r="B135" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C135">
         <v>100</v>
@@ -2303,8 +2312,8 @@
       <c r="A136">
         <v>2115</v>
       </c>
-      <c r="B136">
-        <v>11.11</v>
+      <c r="B136" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C136">
         <v>100</v>
@@ -2317,8 +2326,8 @@
       <c r="A137">
         <v>2116</v>
       </c>
-      <c r="B137">
-        <v>11.11</v>
+      <c r="B137" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C137">
         <v>100</v>
@@ -2331,8 +2340,8 @@
       <c r="A138">
         <v>2117</v>
       </c>
-      <c r="B138">
-        <v>11.11</v>
+      <c r="B138" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C138">
         <v>100</v>
@@ -2345,8 +2354,8 @@
       <c r="A139">
         <v>2118</v>
       </c>
-      <c r="B139">
-        <v>11.11</v>
+      <c r="B139" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C139">
         <v>100</v>
@@ -2359,8 +2368,8 @@
       <c r="A140">
         <v>2119</v>
       </c>
-      <c r="B140">
-        <v>11.11</v>
+      <c r="B140" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C140">
         <v>100</v>
@@ -2370,16 +2379,16 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A141">
+      <c r="A141" s="2">
         <v>2120</v>
       </c>
-      <c r="B141">
-        <v>11.11</v>
-      </c>
-      <c r="C141">
+      <c r="B141" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C141" s="2">
         <v>-1</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2387,8 +2396,8 @@
       <c r="A142">
         <v>2201</v>
       </c>
-      <c r="B142">
-        <v>11.11</v>
+      <c r="B142" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C142">
         <v>100</v>
@@ -2401,8 +2410,8 @@
       <c r="A143">
         <v>2202</v>
       </c>
-      <c r="B143">
-        <v>11.11</v>
+      <c r="B143" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C143">
         <v>100</v>
@@ -2415,8 +2424,8 @@
       <c r="A144">
         <v>2203</v>
       </c>
-      <c r="B144">
-        <v>11.11</v>
+      <c r="B144" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C144">
         <v>100</v>
@@ -2429,8 +2438,8 @@
       <c r="A145">
         <v>2204</v>
       </c>
-      <c r="B145">
-        <v>11.11</v>
+      <c r="B145" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C145">
         <v>100</v>
@@ -2443,8 +2452,8 @@
       <c r="A146">
         <v>2205</v>
       </c>
-      <c r="B146">
-        <v>11.11</v>
+      <c r="B146" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C146">
         <v>100</v>
@@ -2457,8 +2466,8 @@
       <c r="A147">
         <v>2206</v>
       </c>
-      <c r="B147">
-        <v>11.11</v>
+      <c r="B147" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C147">
         <v>100</v>
@@ -2471,22 +2480,22 @@
       <c r="A148">
         <v>2207</v>
       </c>
-      <c r="B148">
-        <v>11.11</v>
+      <c r="B148" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C148">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D148" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A149">
         <v>2208</v>
       </c>
-      <c r="B149">
-        <v>11.11</v>
+      <c r="B149" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C149">
         <v>100</v>
@@ -2499,8 +2508,8 @@
       <c r="A150">
         <v>2209</v>
       </c>
-      <c r="B150">
-        <v>11.11</v>
+      <c r="B150" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C150">
         <v>100</v>
@@ -2513,8 +2522,8 @@
       <c r="A151">
         <v>2210</v>
       </c>
-      <c r="B151">
-        <v>11.11</v>
+      <c r="B151" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C151">
         <v>100</v>
@@ -2527,8 +2536,8 @@
       <c r="A152">
         <v>2211</v>
       </c>
-      <c r="B152">
-        <v>11.11</v>
+      <c r="B152" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C152">
         <v>100</v>
@@ -2541,8 +2550,8 @@
       <c r="A153">
         <v>2212</v>
       </c>
-      <c r="B153">
-        <v>11.11</v>
+      <c r="B153" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C153">
         <v>100</v>
@@ -2555,8 +2564,8 @@
       <c r="A154">
         <v>2213</v>
       </c>
-      <c r="B154">
-        <v>11.11</v>
+      <c r="B154" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C154">
         <v>100</v>
@@ -2569,8 +2578,8 @@
       <c r="A155">
         <v>2214</v>
       </c>
-      <c r="B155">
-        <v>11.11</v>
+      <c r="B155" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C155">
         <v>100</v>
@@ -2583,22 +2592,22 @@
       <c r="A156">
         <v>2215</v>
       </c>
-      <c r="B156">
-        <v>11.11</v>
+      <c r="B156" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C156">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D156" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A157">
         <v>2216</v>
       </c>
-      <c r="B157">
-        <v>11.11</v>
+      <c r="B157" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C157">
         <v>100</v>
@@ -2611,8 +2620,8 @@
       <c r="A158">
         <v>2217</v>
       </c>
-      <c r="B158">
-        <v>11.11</v>
+      <c r="B158" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C158">
         <v>100</v>
@@ -2625,8 +2634,8 @@
       <c r="A159">
         <v>2218</v>
       </c>
-      <c r="B159">
-        <v>11.11</v>
+      <c r="B159" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C159">
         <v>100</v>
@@ -2639,8 +2648,8 @@
       <c r="A160">
         <v>2219</v>
       </c>
-      <c r="B160">
-        <v>11.11</v>
+      <c r="B160" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C160">
         <v>100</v>
@@ -2650,16 +2659,16 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A161">
+      <c r="A161" s="2">
         <v>2220</v>
       </c>
-      <c r="B161">
-        <v>11.11</v>
-      </c>
-      <c r="C161">
+      <c r="B161" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C161" s="2">
         <v>-1</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2667,8 +2676,8 @@
       <c r="A162">
         <v>2301</v>
       </c>
-      <c r="B162">
-        <v>11.11</v>
+      <c r="B162" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C162">
         <v>100</v>
@@ -2681,8 +2690,8 @@
       <c r="A163">
         <v>2302</v>
       </c>
-      <c r="B163">
-        <v>11.11</v>
+      <c r="B163" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C163">
         <v>100</v>
@@ -2692,16 +2701,16 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A164">
+      <c r="A164" s="2">
         <v>2303</v>
       </c>
-      <c r="B164">
-        <v>11.11</v>
-      </c>
-      <c r="C164">
+      <c r="B164" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C164" s="2">
         <v>-1</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2709,8 +2718,8 @@
       <c r="A165">
         <v>2304</v>
       </c>
-      <c r="B165">
-        <v>11.11</v>
+      <c r="B165" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C165">
         <v>100</v>
@@ -2723,8 +2732,8 @@
       <c r="A166">
         <v>2305</v>
       </c>
-      <c r="B166">
-        <v>11.11</v>
+      <c r="B166" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C166">
         <v>100</v>
@@ -2737,8 +2746,8 @@
       <c r="A167">
         <v>2306</v>
       </c>
-      <c r="B167">
-        <v>11.11</v>
+      <c r="B167" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C167">
         <v>100</v>
@@ -2751,8 +2760,8 @@
       <c r="A168">
         <v>2307</v>
       </c>
-      <c r="B168">
-        <v>11.11</v>
+      <c r="B168" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C168">
         <v>100</v>
@@ -2765,8 +2774,8 @@
       <c r="A169">
         <v>2308</v>
       </c>
-      <c r="B169">
-        <v>11.11</v>
+      <c r="B169" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C169">
         <v>100</v>
@@ -2779,8 +2788,8 @@
       <c r="A170">
         <v>2309</v>
       </c>
-      <c r="B170">
-        <v>11.11</v>
+      <c r="B170" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C170">
         <v>100</v>
@@ -2793,22 +2802,22 @@
       <c r="A171">
         <v>2310</v>
       </c>
-      <c r="B171">
-        <v>11.11</v>
+      <c r="B171" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C171">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D171" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A172">
         <v>2311</v>
       </c>
-      <c r="B172">
-        <v>11.11</v>
+      <c r="B172" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C172">
         <v>100</v>
@@ -2821,8 +2830,8 @@
       <c r="A173">
         <v>2312</v>
       </c>
-      <c r="B173">
-        <v>11.11</v>
+      <c r="B173" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C173">
         <v>100</v>
@@ -2835,8 +2844,8 @@
       <c r="A174">
         <v>2313</v>
       </c>
-      <c r="B174">
-        <v>11.11</v>
+      <c r="B174" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C174">
         <v>100</v>
@@ -2849,8 +2858,8 @@
       <c r="A175">
         <v>2314</v>
       </c>
-      <c r="B175">
-        <v>11.11</v>
+      <c r="B175" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C175">
         <v>100</v>
@@ -2863,8 +2872,8 @@
       <c r="A176">
         <v>2315</v>
       </c>
-      <c r="B176">
-        <v>11.11</v>
+      <c r="B176" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C176">
         <v>100</v>
@@ -2877,8 +2886,8 @@
       <c r="A177">
         <v>2316</v>
       </c>
-      <c r="B177">
-        <v>11.11</v>
+      <c r="B177" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C177">
         <v>100</v>
@@ -2891,55 +2900,55 @@
       <c r="A178">
         <v>2317</v>
       </c>
-      <c r="B178">
-        <v>11.11</v>
+      <c r="B178" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C178">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D178" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A179">
+      <c r="A179" s="2">
         <v>2318</v>
       </c>
-      <c r="B179">
-        <v>11.11</v>
-      </c>
-      <c r="C179">
+      <c r="B179" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C179" s="2">
         <v>-1</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A180">
+      <c r="A180" s="2">
         <v>2319</v>
       </c>
-      <c r="B180">
-        <v>11.11</v>
-      </c>
-      <c r="C180">
+      <c r="B180" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C180" s="2">
         <v>-1</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A181">
+      <c r="A181" s="2">
         <v>2320</v>
       </c>
-      <c r="B181">
-        <v>11.11</v>
-      </c>
-      <c r="C181">
+      <c r="B181" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C181" s="2">
         <v>-1</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2947,8 +2956,8 @@
       <c r="A182">
         <v>2401</v>
       </c>
-      <c r="B182">
-        <v>11.11</v>
+      <c r="B182" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C182">
         <v>100</v>
@@ -2961,8 +2970,8 @@
       <c r="A183">
         <v>2402</v>
       </c>
-      <c r="B183">
-        <v>11.11</v>
+      <c r="B183" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C183">
         <v>100</v>
@@ -2975,22 +2984,22 @@
       <c r="A184">
         <v>2403</v>
       </c>
-      <c r="B184">
-        <v>11.11</v>
+      <c r="B184" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C184">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D184" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A185">
         <v>2404</v>
       </c>
-      <c r="B185">
-        <v>11.11</v>
+      <c r="B185" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C185">
         <v>100</v>
@@ -3003,8 +3012,8 @@
       <c r="A186">
         <v>2405</v>
       </c>
-      <c r="B186">
-        <v>11.11</v>
+      <c r="B186" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C186">
         <v>100</v>
@@ -3017,8 +3026,8 @@
       <c r="A187">
         <v>2406</v>
       </c>
-      <c r="B187">
-        <v>11.11</v>
+      <c r="B187" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C187">
         <v>100</v>
@@ -3028,16 +3037,16 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A188">
+      <c r="A188" s="2">
         <v>2407</v>
       </c>
-      <c r="B188">
-        <v>11.11</v>
-      </c>
-      <c r="C188">
+      <c r="B188" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C188" s="2">
         <v>-1</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3045,11 +3054,11 @@
       <c r="A189">
         <v>2408</v>
       </c>
-      <c r="B189">
-        <v>11.11</v>
+      <c r="B189" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C189">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D189" t="s">
         <v>4</v>
@@ -3059,22 +3068,22 @@
       <c r="A190">
         <v>2409</v>
       </c>
-      <c r="B190">
-        <v>11.11</v>
+      <c r="B190" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C190">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D190" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A191">
         <v>2410</v>
       </c>
-      <c r="B191">
-        <v>11.11</v>
+      <c r="B191" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C191">
         <v>100</v>
@@ -3087,8 +3096,8 @@
       <c r="A192">
         <v>2411</v>
       </c>
-      <c r="B192">
-        <v>11.11</v>
+      <c r="B192" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C192">
         <v>100</v>
@@ -3101,8 +3110,8 @@
       <c r="A193">
         <v>2412</v>
       </c>
-      <c r="B193">
-        <v>11.11</v>
+      <c r="B193" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C193">
         <v>100</v>
@@ -3115,8 +3124,8 @@
       <c r="A194">
         <v>2413</v>
       </c>
-      <c r="B194">
-        <v>11.11</v>
+      <c r="B194" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C194">
         <v>100</v>
@@ -3129,8 +3138,8 @@
       <c r="A195">
         <v>2414</v>
       </c>
-      <c r="B195">
-        <v>11.11</v>
+      <c r="B195" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C195">
         <v>100</v>
@@ -3143,8 +3152,8 @@
       <c r="A196">
         <v>2415</v>
       </c>
-      <c r="B196">
-        <v>11.11</v>
+      <c r="B196" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C196">
         <v>100</v>
@@ -3157,22 +3166,22 @@
       <c r="A197">
         <v>2416</v>
       </c>
-      <c r="B197">
-        <v>11.11</v>
+      <c r="B197" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C197">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D197" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A198">
         <v>2417</v>
       </c>
-      <c r="B198">
-        <v>11.11</v>
+      <c r="B198" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C198">
         <v>100</v>
@@ -3182,44 +3191,44 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A199">
+      <c r="A199" s="2">
         <v>2418</v>
       </c>
-      <c r="B199">
-        <v>11.11</v>
-      </c>
-      <c r="C199">
+      <c r="B199" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C199" s="2">
         <v>-1</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A200">
+      <c r="A200" s="2">
         <v>2419</v>
       </c>
-      <c r="B200">
-        <v>11.11</v>
-      </c>
-      <c r="C200">
+      <c r="B200" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C200" s="2">
         <v>-1</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A201">
+      <c r="A201" s="2">
         <v>2420</v>
       </c>
-      <c r="B201">
-        <v>11.11</v>
-      </c>
-      <c r="C201">
+      <c r="B201" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C201" s="2">
         <v>-1</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3227,8 +3236,8 @@
       <c r="A202">
         <v>2501</v>
       </c>
-      <c r="B202">
-        <v>11.11</v>
+      <c r="B202" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C202">
         <v>100</v>
@@ -3241,8 +3250,8 @@
       <c r="A203">
         <v>2502</v>
       </c>
-      <c r="B203">
-        <v>11.11</v>
+      <c r="B203" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C203">
         <v>100</v>
@@ -3255,8 +3264,8 @@
       <c r="A204">
         <v>2503</v>
       </c>
-      <c r="B204">
-        <v>11.11</v>
+      <c r="B204" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C204">
         <v>100</v>
@@ -3269,8 +3278,8 @@
       <c r="A205">
         <v>2504</v>
       </c>
-      <c r="B205">
-        <v>11.11</v>
+      <c r="B205" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C205">
         <v>100</v>
@@ -3283,8 +3292,8 @@
       <c r="A206">
         <v>2505</v>
       </c>
-      <c r="B206">
-        <v>11.11</v>
+      <c r="B206" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C206">
         <v>100</v>
@@ -3297,8 +3306,8 @@
       <c r="A207">
         <v>2506</v>
       </c>
-      <c r="B207">
-        <v>11.11</v>
+      <c r="B207" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C207">
         <v>100</v>
@@ -3311,8 +3320,8 @@
       <c r="A208">
         <v>2507</v>
       </c>
-      <c r="B208">
-        <v>11.11</v>
+      <c r="B208" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C208">
         <v>100</v>
@@ -3325,8 +3334,8 @@
       <c r="A209">
         <v>2508</v>
       </c>
-      <c r="B209">
-        <v>11.11</v>
+      <c r="B209" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C209">
         <v>100</v>
@@ -3339,8 +3348,8 @@
       <c r="A210">
         <v>2509</v>
       </c>
-      <c r="B210">
-        <v>11.11</v>
+      <c r="B210" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C210">
         <v>100</v>
@@ -3353,8 +3362,8 @@
       <c r="A211">
         <v>2510</v>
       </c>
-      <c r="B211">
-        <v>11.11</v>
+      <c r="B211" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C211">
         <v>100</v>
@@ -3367,8 +3376,8 @@
       <c r="A212">
         <v>2511</v>
       </c>
-      <c r="B212">
-        <v>11.11</v>
+      <c r="B212" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C212">
         <v>100</v>
@@ -3381,8 +3390,8 @@
       <c r="A213">
         <v>2512</v>
       </c>
-      <c r="B213">
-        <v>11.11</v>
+      <c r="B213" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C213">
         <v>100</v>
@@ -3395,22 +3404,22 @@
       <c r="A214">
         <v>2513</v>
       </c>
-      <c r="B214">
-        <v>11.11</v>
+      <c r="B214" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C214">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D214" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A215">
         <v>2514</v>
       </c>
-      <c r="B215">
-        <v>11.11</v>
+      <c r="B215" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C215">
         <v>100</v>
@@ -3423,8 +3432,8 @@
       <c r="A216">
         <v>2515</v>
       </c>
-      <c r="B216">
-        <v>11.11</v>
+      <c r="B216" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C216">
         <v>100</v>
@@ -3437,8 +3446,8 @@
       <c r="A217">
         <v>2516</v>
       </c>
-      <c r="B217">
-        <v>11.11</v>
+      <c r="B217" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C217">
         <v>100</v>
@@ -3451,8 +3460,8 @@
       <c r="A218">
         <v>2517</v>
       </c>
-      <c r="B218">
-        <v>11.11</v>
+      <c r="B218" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C218">
         <v>100</v>
@@ -3465,8 +3474,8 @@
       <c r="A219">
         <v>2518</v>
       </c>
-      <c r="B219">
-        <v>11.11</v>
+      <c r="B219" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C219">
         <v>100</v>
@@ -3479,8 +3488,8 @@
       <c r="A220">
         <v>2519</v>
       </c>
-      <c r="B220">
-        <v>11.11</v>
+      <c r="B220" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C220">
         <v>100</v>
@@ -3490,16 +3499,16 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A221">
+      <c r="A221" s="2">
         <v>2520</v>
       </c>
-      <c r="B221">
-        <v>11.11</v>
-      </c>
-      <c r="C221">
+      <c r="B221" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C221" s="2">
         <v>-1</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3507,8 +3516,8 @@
       <c r="A222">
         <v>2601</v>
       </c>
-      <c r="B222">
-        <v>11.11</v>
+      <c r="B222" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C222">
         <v>100</v>
@@ -3521,8 +3530,8 @@
       <c r="A223">
         <v>2602</v>
       </c>
-      <c r="B223">
-        <v>11.11</v>
+      <c r="B223" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C223">
         <v>100</v>
@@ -3535,8 +3544,8 @@
       <c r="A224">
         <v>2603</v>
       </c>
-      <c r="B224">
-        <v>11.11</v>
+      <c r="B224" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C224">
         <v>100</v>
@@ -3549,8 +3558,8 @@
       <c r="A225">
         <v>2604</v>
       </c>
-      <c r="B225">
-        <v>11.11</v>
+      <c r="B225" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C225">
         <v>100</v>
@@ -3563,22 +3572,22 @@
       <c r="A226">
         <v>2605</v>
       </c>
-      <c r="B226">
-        <v>11.11</v>
+      <c r="B226" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C226">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D226" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A227">
         <v>2606</v>
       </c>
-      <c r="B227">
-        <v>11.11</v>
+      <c r="B227" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C227">
         <v>100</v>
@@ -3588,16 +3597,16 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A228">
+      <c r="A228" s="2">
         <v>2607</v>
       </c>
-      <c r="B228">
-        <v>11.11</v>
-      </c>
-      <c r="C228">
+      <c r="B228" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C228" s="2">
         <v>-1</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3605,8 +3614,8 @@
       <c r="A229">
         <v>2608</v>
       </c>
-      <c r="B229">
-        <v>11.11</v>
+      <c r="B229" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C229">
         <v>100</v>
@@ -3619,8 +3628,8 @@
       <c r="A230">
         <v>2609</v>
       </c>
-      <c r="B230">
-        <v>11.11</v>
+      <c r="B230" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C230">
         <v>100</v>
@@ -3633,8 +3642,8 @@
       <c r="A231">
         <v>2610</v>
       </c>
-      <c r="B231">
-        <v>11.11</v>
+      <c r="B231" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C231">
         <v>100</v>
@@ -3647,22 +3656,22 @@
       <c r="A232">
         <v>2611</v>
       </c>
-      <c r="B232">
-        <v>11.11</v>
+      <c r="B232" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C232">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D232" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A233">
         <v>2612</v>
       </c>
-      <c r="B233">
-        <v>11.11</v>
+      <c r="B233" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C233">
         <v>100</v>
@@ -3675,8 +3684,8 @@
       <c r="A234">
         <v>2613</v>
       </c>
-      <c r="B234">
-        <v>11.11</v>
+      <c r="B234" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C234">
         <v>100</v>
@@ -3689,8 +3698,8 @@
       <c r="A235">
         <v>2614</v>
       </c>
-      <c r="B235">
-        <v>11.11</v>
+      <c r="B235" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C235">
         <v>100</v>
@@ -3703,8 +3712,8 @@
       <c r="A236">
         <v>2615</v>
       </c>
-      <c r="B236">
-        <v>11.11</v>
+      <c r="B236" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C236">
         <v>100</v>
@@ -3717,8 +3726,8 @@
       <c r="A237">
         <v>2616</v>
       </c>
-      <c r="B237">
-        <v>11.11</v>
+      <c r="B237" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C237">
         <v>100</v>
@@ -3731,8 +3740,8 @@
       <c r="A238">
         <v>2617</v>
       </c>
-      <c r="B238">
-        <v>11.11</v>
+      <c r="B238" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C238">
         <v>100</v>
@@ -3745,8 +3754,8 @@
       <c r="A239">
         <v>2618</v>
       </c>
-      <c r="B239">
-        <v>11.11</v>
+      <c r="B239" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C239">
         <v>100</v>
@@ -3759,8 +3768,8 @@
       <c r="A240">
         <v>2619</v>
       </c>
-      <c r="B240">
-        <v>11.11</v>
+      <c r="B240" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C240">
         <v>100</v>
@@ -3770,16 +3779,16 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A241">
+      <c r="A241" s="2">
         <v>2620</v>
       </c>
-      <c r="B241">
-        <v>11.11</v>
-      </c>
-      <c r="C241">
+      <c r="B241" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C241" s="2">
         <v>-1</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3787,8 +3796,8 @@
       <c r="A242">
         <v>3101</v>
       </c>
-      <c r="B242">
-        <v>11.11</v>
+      <c r="B242" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C242">
         <v>100</v>
@@ -3801,8 +3810,8 @@
       <c r="A243">
         <v>3102</v>
       </c>
-      <c r="B243">
-        <v>11.11</v>
+      <c r="B243" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C243">
         <v>100</v>
@@ -3815,8 +3824,8 @@
       <c r="A244">
         <v>3103</v>
       </c>
-      <c r="B244">
-        <v>11.11</v>
+      <c r="B244" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C244">
         <v>100</v>
@@ -3829,8 +3838,8 @@
       <c r="A245">
         <v>3104</v>
       </c>
-      <c r="B245">
-        <v>11.11</v>
+      <c r="B245" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C245">
         <v>100</v>
@@ -3843,8 +3852,8 @@
       <c r="A246">
         <v>3105</v>
       </c>
-      <c r="B246">
-        <v>11.11</v>
+      <c r="B246" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C246">
         <v>100</v>
@@ -3857,8 +3866,8 @@
       <c r="A247">
         <v>3106</v>
       </c>
-      <c r="B247">
-        <v>11.11</v>
+      <c r="B247" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C247">
         <v>100</v>
@@ -3871,8 +3880,8 @@
       <c r="A248">
         <v>3107</v>
       </c>
-      <c r="B248">
-        <v>11.11</v>
+      <c r="B248" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C248">
         <v>100</v>
@@ -3885,11 +3894,11 @@
       <c r="A249">
         <v>3108</v>
       </c>
-      <c r="B249">
-        <v>11.11</v>
+      <c r="B249" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C249">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D249" t="s">
         <v>4</v>
@@ -3899,22 +3908,22 @@
       <c r="A250">
         <v>3109</v>
       </c>
-      <c r="B250">
-        <v>11.11</v>
+      <c r="B250" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C250">
         <v>100</v>
       </c>
       <c r="D250" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A251">
         <v>3110</v>
       </c>
-      <c r="B251">
-        <v>11.11</v>
+      <c r="B251" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C251">
         <v>100</v>
@@ -3927,8 +3936,8 @@
       <c r="A252">
         <v>3111</v>
       </c>
-      <c r="B252">
-        <v>11.11</v>
+      <c r="B252" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C252">
         <v>100</v>
@@ -3941,22 +3950,22 @@
       <c r="A253">
         <v>3112</v>
       </c>
-      <c r="B253">
-        <v>11.11</v>
+      <c r="B253" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C253">
         <v>100</v>
       </c>
       <c r="D253" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A254">
         <v>3113</v>
       </c>
-      <c r="B254">
-        <v>11.11</v>
+      <c r="B254" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C254">
         <v>100</v>
@@ -3969,8 +3978,8 @@
       <c r="A255">
         <v>3114</v>
       </c>
-      <c r="B255">
-        <v>11.11</v>
+      <c r="B255" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C255">
         <v>100</v>
@@ -3983,8 +3992,8 @@
       <c r="A256">
         <v>3115</v>
       </c>
-      <c r="B256">
-        <v>11.11</v>
+      <c r="B256" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C256">
         <v>100</v>
@@ -3997,8 +4006,8 @@
       <c r="A257">
         <v>3116</v>
       </c>
-      <c r="B257">
-        <v>11.11</v>
+      <c r="B257" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C257">
         <v>100</v>
@@ -4011,8 +4020,8 @@
       <c r="A258">
         <v>3117</v>
       </c>
-      <c r="B258">
-        <v>11.11</v>
+      <c r="B258" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C258">
         <v>100</v>
@@ -4025,8 +4034,8 @@
       <c r="A259">
         <v>3118</v>
       </c>
-      <c r="B259">
-        <v>11.11</v>
+      <c r="B259" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C259">
         <v>100</v>
@@ -4039,8 +4048,8 @@
       <c r="A260">
         <v>3119</v>
       </c>
-      <c r="B260">
-        <v>11.11</v>
+      <c r="B260" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C260">
         <v>100</v>
@@ -4050,16 +4059,16 @@
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A261">
+      <c r="A261" s="2">
         <v>3120</v>
       </c>
-      <c r="B261">
-        <v>11.11</v>
-      </c>
-      <c r="C261">
+      <c r="B261" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C261" s="2">
         <v>-1</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D261" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4067,8 +4076,8 @@
       <c r="A262">
         <v>3201</v>
       </c>
-      <c r="B262">
-        <v>11.11</v>
+      <c r="B262" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C262">
         <v>100</v>
@@ -4081,8 +4090,8 @@
       <c r="A263">
         <v>3202</v>
       </c>
-      <c r="B263">
-        <v>11.11</v>
+      <c r="B263" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C263">
         <v>100</v>
@@ -4095,11 +4104,11 @@
       <c r="A264">
         <v>3203</v>
       </c>
-      <c r="B264">
-        <v>11.11</v>
+      <c r="B264" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C264">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D264" t="s">
         <v>4</v>
@@ -4109,8 +4118,8 @@
       <c r="A265">
         <v>3204</v>
       </c>
-      <c r="B265">
-        <v>11.11</v>
+      <c r="B265" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C265">
         <v>100</v>
@@ -4123,8 +4132,8 @@
       <c r="A266">
         <v>3205</v>
       </c>
-      <c r="B266">
-        <v>11.11</v>
+      <c r="B266" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C266">
         <v>100</v>
@@ -4137,8 +4146,8 @@
       <c r="A267">
         <v>3206</v>
       </c>
-      <c r="B267">
-        <v>11.11</v>
+      <c r="B267" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C267">
         <v>100</v>
@@ -4151,22 +4160,22 @@
       <c r="A268">
         <v>3207</v>
       </c>
-      <c r="B268">
-        <v>11.11</v>
+      <c r="B268" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C268">
         <v>100</v>
       </c>
       <c r="D268" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A269">
         <v>3208</v>
       </c>
-      <c r="B269">
-        <v>11.11</v>
+      <c r="B269" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C269">
         <v>100</v>
@@ -4179,8 +4188,8 @@
       <c r="A270">
         <v>3209</v>
       </c>
-      <c r="B270">
-        <v>11.11</v>
+      <c r="B270" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C270">
         <v>100</v>
@@ -4193,8 +4202,8 @@
       <c r="A271">
         <v>3210</v>
       </c>
-      <c r="B271">
-        <v>11.11</v>
+      <c r="B271" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C271">
         <v>100</v>
@@ -4207,8 +4216,8 @@
       <c r="A272">
         <v>3211</v>
       </c>
-      <c r="B272">
-        <v>11.11</v>
+      <c r="B272" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C272">
         <v>100</v>
@@ -4221,8 +4230,8 @@
       <c r="A273">
         <v>3212</v>
       </c>
-      <c r="B273">
-        <v>11.11</v>
+      <c r="B273" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C273">
         <v>100</v>
@@ -4235,8 +4244,8 @@
       <c r="A274">
         <v>3213</v>
       </c>
-      <c r="B274">
-        <v>11.11</v>
+      <c r="B274" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C274">
         <v>100</v>
@@ -4249,8 +4258,8 @@
       <c r="A275">
         <v>3214</v>
       </c>
-      <c r="B275">
-        <v>11.11</v>
+      <c r="B275" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C275">
         <v>100</v>
@@ -4263,22 +4272,22 @@
       <c r="A276">
         <v>3215</v>
       </c>
-      <c r="B276">
-        <v>11.11</v>
+      <c r="B276" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C276">
         <v>100</v>
       </c>
       <c r="D276" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A277">
         <v>3216</v>
       </c>
-      <c r="B277">
-        <v>11.11</v>
+      <c r="B277" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C277">
         <v>100</v>
@@ -4291,11 +4300,11 @@
       <c r="A278">
         <v>3217</v>
       </c>
-      <c r="B278">
-        <v>11.11</v>
+      <c r="B278" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C278">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D278" t="s">
         <v>4</v>
@@ -4305,8 +4314,8 @@
       <c r="A279">
         <v>3218</v>
       </c>
-      <c r="B279">
-        <v>11.11</v>
+      <c r="B279" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C279">
         <v>100</v>
@@ -4316,30 +4325,30 @@
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A280">
+      <c r="A280" s="2">
         <v>3219</v>
       </c>
-      <c r="B280">
-        <v>11.11</v>
-      </c>
-      <c r="C280">
+      <c r="B280" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C280" s="2">
         <v>-1</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A281">
+      <c r="A281" s="2">
         <v>3220</v>
       </c>
-      <c r="B281">
-        <v>11.11</v>
-      </c>
-      <c r="C281">
+      <c r="B281" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C281" s="2">
         <v>-1</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4347,8 +4356,8 @@
       <c r="A282">
         <v>3301</v>
       </c>
-      <c r="B282">
-        <v>11.11</v>
+      <c r="B282" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C282">
         <v>100</v>
@@ -4361,8 +4370,8 @@
       <c r="A283">
         <v>3302</v>
       </c>
-      <c r="B283">
-        <v>11.11</v>
+      <c r="B283" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C283">
         <v>100</v>
@@ -4375,8 +4384,8 @@
       <c r="A284">
         <v>3303</v>
       </c>
-      <c r="B284">
-        <v>11.11</v>
+      <c r="B284" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C284">
         <v>100</v>
@@ -4389,8 +4398,8 @@
       <c r="A285">
         <v>3304</v>
       </c>
-      <c r="B285">
-        <v>11.11</v>
+      <c r="B285" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C285">
         <v>100</v>
@@ -4403,8 +4412,8 @@
       <c r="A286">
         <v>3305</v>
       </c>
-      <c r="B286">
-        <v>11.11</v>
+      <c r="B286" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C286">
         <v>100</v>
@@ -4417,8 +4426,8 @@
       <c r="A287">
         <v>3306</v>
       </c>
-      <c r="B287">
-        <v>11.11</v>
+      <c r="B287" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C287">
         <v>100</v>
@@ -4431,8 +4440,8 @@
       <c r="A288">
         <v>3307</v>
       </c>
-      <c r="B288">
-        <v>11.11</v>
+      <c r="B288" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C288">
         <v>100</v>
@@ -4445,8 +4454,8 @@
       <c r="A289">
         <v>3308</v>
       </c>
-      <c r="B289">
-        <v>11.11</v>
+      <c r="B289" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C289">
         <v>100</v>
@@ -4459,8 +4468,8 @@
       <c r="A290">
         <v>3309</v>
       </c>
-      <c r="B290">
-        <v>11.11</v>
+      <c r="B290" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C290">
         <v>100</v>
@@ -4473,22 +4482,22 @@
       <c r="A291">
         <v>3310</v>
       </c>
-      <c r="B291">
-        <v>11.11</v>
+      <c r="B291" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C291">
         <v>100</v>
       </c>
       <c r="D291" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A292">
         <v>3311</v>
       </c>
-      <c r="B292">
-        <v>11.11</v>
+      <c r="B292" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C292">
         <v>100</v>
@@ -4501,11 +4510,11 @@
       <c r="A293">
         <v>3312</v>
       </c>
-      <c r="B293">
-        <v>11.11</v>
+      <c r="B293" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C293">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D293" t="s">
         <v>4</v>
@@ -4515,8 +4524,8 @@
       <c r="A294">
         <v>3313</v>
       </c>
-      <c r="B294">
-        <v>11.11</v>
+      <c r="B294" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C294">
         <v>100</v>
@@ -4529,8 +4538,8 @@
       <c r="A295">
         <v>3314</v>
       </c>
-      <c r="B295">
-        <v>11.11</v>
+      <c r="B295" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C295">
         <v>100</v>
@@ -4543,8 +4552,8 @@
       <c r="A296">
         <v>3315</v>
       </c>
-      <c r="B296">
-        <v>11.11</v>
+      <c r="B296" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C296">
         <v>100</v>
@@ -4557,8 +4566,8 @@
       <c r="A297">
         <v>3316</v>
       </c>
-      <c r="B297">
-        <v>11.11</v>
+      <c r="B297" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C297">
         <v>100</v>
@@ -4571,22 +4580,22 @@
       <c r="A298">
         <v>3317</v>
       </c>
-      <c r="B298">
-        <v>11.11</v>
+      <c r="B298" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C298">
         <v>100</v>
       </c>
       <c r="D298" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A299">
         <v>3318</v>
       </c>
-      <c r="B299">
-        <v>11.11</v>
+      <c r="B299" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C299">
         <v>100</v>
@@ -4596,30 +4605,30 @@
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A300">
+      <c r="A300" s="2">
         <v>3319</v>
       </c>
-      <c r="B300">
-        <v>11.11</v>
-      </c>
-      <c r="C300">
+      <c r="B300" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C300" s="2">
         <v>-1</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D300" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A301">
+      <c r="A301" s="2">
         <v>3320</v>
       </c>
-      <c r="B301">
-        <v>11.11</v>
-      </c>
-      <c r="C301">
+      <c r="B301" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C301" s="2">
         <v>-1</v>
       </c>
-      <c r="D301" t="s">
+      <c r="D301" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4627,8 +4636,8 @@
       <c r="A302">
         <v>3401</v>
       </c>
-      <c r="B302">
-        <v>11.11</v>
+      <c r="B302" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C302">
         <v>100</v>
@@ -4641,8 +4650,8 @@
       <c r="A303">
         <v>3402</v>
       </c>
-      <c r="B303">
-        <v>11.11</v>
+      <c r="B303" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C303">
         <v>100</v>
@@ -4655,25 +4664,25 @@
       <c r="A304">
         <v>3403</v>
       </c>
-      <c r="B304">
-        <v>11.11</v>
+      <c r="B304" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C304">
         <v>100</v>
       </c>
       <c r="D304" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A305">
         <v>3404</v>
       </c>
-      <c r="B305">
-        <v>11.11</v>
+      <c r="B305" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C305">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D305" t="s">
         <v>4</v>
@@ -4683,8 +4692,8 @@
       <c r="A306">
         <v>3405</v>
       </c>
-      <c r="B306">
-        <v>11.11</v>
+      <c r="B306" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C306">
         <v>100</v>
@@ -4697,8 +4706,8 @@
       <c r="A307">
         <v>3406</v>
       </c>
-      <c r="B307">
-        <v>11.11</v>
+      <c r="B307" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C307">
         <v>100</v>
@@ -4711,11 +4720,11 @@
       <c r="A308">
         <v>3407</v>
       </c>
-      <c r="B308">
-        <v>11.11</v>
+      <c r="B308" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C308">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D308" t="s">
         <v>4</v>
@@ -4725,8 +4734,8 @@
       <c r="A309">
         <v>3408</v>
       </c>
-      <c r="B309">
-        <v>11.11</v>
+      <c r="B309" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C309">
         <v>100</v>
@@ -4739,22 +4748,22 @@
       <c r="A310">
         <v>3409</v>
       </c>
-      <c r="B310">
-        <v>11.11</v>
+      <c r="B310" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C310">
         <v>100</v>
       </c>
       <c r="D310" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A311">
         <v>3410</v>
       </c>
-      <c r="B311">
-        <v>11.11</v>
+      <c r="B311" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C311">
         <v>100</v>
@@ -4767,8 +4776,8 @@
       <c r="A312">
         <v>3411</v>
       </c>
-      <c r="B312">
-        <v>11.11</v>
+      <c r="B312" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C312">
         <v>100</v>
@@ -4781,8 +4790,8 @@
       <c r="A313">
         <v>3412</v>
       </c>
-      <c r="B313">
-        <v>11.11</v>
+      <c r="B313" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C313">
         <v>100</v>
@@ -4795,8 +4804,8 @@
       <c r="A314">
         <v>3413</v>
       </c>
-      <c r="B314">
-        <v>11.11</v>
+      <c r="B314" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C314">
         <v>100</v>
@@ -4809,8 +4818,8 @@
       <c r="A315">
         <v>3414</v>
       </c>
-      <c r="B315">
-        <v>11.11</v>
+      <c r="B315" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C315">
         <v>100</v>
@@ -4823,8 +4832,8 @@
       <c r="A316">
         <v>3415</v>
       </c>
-      <c r="B316">
-        <v>11.11</v>
+      <c r="B316" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C316">
         <v>100</v>
@@ -4837,22 +4846,22 @@
       <c r="A317">
         <v>3416</v>
       </c>
-      <c r="B317">
-        <v>11.11</v>
+      <c r="B317" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C317">
         <v>100</v>
       </c>
       <c r="D317" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A318">
         <v>3417</v>
       </c>
-      <c r="B318">
-        <v>11.11</v>
+      <c r="B318" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C318">
         <v>100</v>
@@ -4865,8 +4874,8 @@
       <c r="A319">
         <v>3418</v>
       </c>
-      <c r="B319">
-        <v>11.11</v>
+      <c r="B319" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C319">
         <v>100</v>
@@ -4876,30 +4885,30 @@
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A320">
+      <c r="A320" s="2">
         <v>3419</v>
       </c>
-      <c r="B320">
-        <v>11.11</v>
-      </c>
-      <c r="C320">
+      <c r="B320" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C320" s="2">
         <v>-1</v>
       </c>
-      <c r="D320" t="s">
+      <c r="D320" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A321">
+      <c r="A321" s="2">
         <v>3420</v>
       </c>
-      <c r="B321">
-        <v>11.11</v>
-      </c>
-      <c r="C321">
+      <c r="B321" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C321" s="2">
         <v>-1</v>
       </c>
-      <c r="D321" t="s">
+      <c r="D321" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4907,8 +4916,8 @@
       <c r="A322">
         <v>3501</v>
       </c>
-      <c r="B322">
-        <v>11.11</v>
+      <c r="B322" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C322">
         <v>100</v>
@@ -4921,8 +4930,8 @@
       <c r="A323">
         <v>3502</v>
       </c>
-      <c r="B323">
-        <v>11.11</v>
+      <c r="B323" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C323">
         <v>100</v>
@@ -4935,8 +4944,8 @@
       <c r="A324">
         <v>3503</v>
       </c>
-      <c r="B324">
-        <v>11.11</v>
+      <c r="B324" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C324">
         <v>100</v>
@@ -4949,8 +4958,8 @@
       <c r="A325">
         <v>3504</v>
       </c>
-      <c r="B325">
-        <v>11.11</v>
+      <c r="B325" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C325">
         <v>100</v>
@@ -4963,8 +4972,8 @@
       <c r="A326">
         <v>3505</v>
       </c>
-      <c r="B326">
-        <v>11.11</v>
+      <c r="B326" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C326">
         <v>100</v>
@@ -4977,8 +4986,8 @@
       <c r="A327">
         <v>3506</v>
       </c>
-      <c r="B327">
-        <v>11.11</v>
+      <c r="B327" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C327">
         <v>100</v>
@@ -4991,8 +5000,8 @@
       <c r="A328">
         <v>3507</v>
       </c>
-      <c r="B328">
-        <v>11.11</v>
+      <c r="B328" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C328">
         <v>100</v>
@@ -5005,8 +5014,8 @@
       <c r="A329">
         <v>3508</v>
       </c>
-      <c r="B329">
-        <v>11.11</v>
+      <c r="B329" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C329">
         <v>100</v>
@@ -5019,8 +5028,8 @@
       <c r="A330">
         <v>3509</v>
       </c>
-      <c r="B330">
-        <v>11.11</v>
+      <c r="B330" s="5">
+        <v>44183.375</v>
       </c>
       <c r="C330">
         <v>100</v>
@@ -5033,8 +5042,8 @@
       <c r="A331">
         <v>3510</v>
       </c>
-      <c r="B331">
-        <v>11.11</v>
+      <c r="B331" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C331">
         <v>100</v>
@@ -5047,8 +5056,8 @@
       <c r="A332">
         <v>3511</v>
       </c>
-      <c r="B332">
-        <v>11.11</v>
+      <c r="B332" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C332">
         <v>100</v>
@@ -5061,8 +5070,8 @@
       <c r="A333">
         <v>3512</v>
       </c>
-      <c r="B333">
-        <v>11.11</v>
+      <c r="B333" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C333">
         <v>100</v>
@@ -5075,22 +5084,22 @@
       <c r="A334">
         <v>3513</v>
       </c>
-      <c r="B334">
-        <v>11.11</v>
+      <c r="B334" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C334">
         <v>100</v>
       </c>
       <c r="D334" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A335">
         <v>3514</v>
       </c>
-      <c r="B335">
-        <v>11.11</v>
+      <c r="B335" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C335">
         <v>100</v>
@@ -5103,8 +5112,8 @@
       <c r="A336">
         <v>3515</v>
       </c>
-      <c r="B336">
-        <v>11.11</v>
+      <c r="B336" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C336">
         <v>100</v>
@@ -5117,8 +5126,8 @@
       <c r="A337">
         <v>3516</v>
       </c>
-      <c r="B337">
-        <v>11.11</v>
+      <c r="B337" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C337">
         <v>100</v>
@@ -5131,55 +5140,55 @@
       <c r="A338">
         <v>3517</v>
       </c>
-      <c r="B338">
-        <v>11.11</v>
+      <c r="B338" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C338">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D338" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A339">
+      <c r="A339" s="2">
         <v>3518</v>
       </c>
-      <c r="B339">
-        <v>11.11</v>
-      </c>
-      <c r="C339">
+      <c r="B339" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C339" s="2">
         <v>-1</v>
       </c>
-      <c r="D339" t="s">
+      <c r="D339" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A340">
+      <c r="A340" s="2">
         <v>3519</v>
       </c>
-      <c r="B340">
-        <v>11.11</v>
-      </c>
-      <c r="C340">
+      <c r="B340" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C340" s="2">
         <v>-1</v>
       </c>
-      <c r="D340" t="s">
+      <c r="D340" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A341">
+      <c r="A341" s="2">
         <v>3520</v>
       </c>
-      <c r="B341">
-        <v>11.11</v>
-      </c>
-      <c r="C341">
+      <c r="B341" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C341" s="2">
         <v>-1</v>
       </c>
-      <c r="D341" t="s">
+      <c r="D341" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5187,8 +5196,8 @@
       <c r="A342">
         <v>3601</v>
       </c>
-      <c r="B342">
-        <v>11.11</v>
+      <c r="B342" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C342">
         <v>100</v>
@@ -5201,8 +5210,8 @@
       <c r="A343">
         <v>3602</v>
       </c>
-      <c r="B343">
-        <v>11.11</v>
+      <c r="B343" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C343">
         <v>100</v>
@@ -5215,8 +5224,8 @@
       <c r="A344">
         <v>3603</v>
       </c>
-      <c r="B344">
-        <v>11.11</v>
+      <c r="B344" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C344">
         <v>100</v>
@@ -5229,8 +5238,8 @@
       <c r="A345">
         <v>3604</v>
       </c>
-      <c r="B345">
-        <v>11.11</v>
+      <c r="B345" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C345">
         <v>100</v>
@@ -5243,22 +5252,22 @@
       <c r="A346">
         <v>3605</v>
       </c>
-      <c r="B346">
-        <v>11.11</v>
+      <c r="B346" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C346">
         <v>100</v>
       </c>
       <c r="D346" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A347">
         <v>3606</v>
       </c>
-      <c r="B347">
-        <v>11.11</v>
+      <c r="B347" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C347">
         <v>100</v>
@@ -5271,8 +5280,8 @@
       <c r="A348">
         <v>3607</v>
       </c>
-      <c r="B348">
-        <v>11.11</v>
+      <c r="B348" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C348">
         <v>100</v>
@@ -5285,8 +5294,8 @@
       <c r="A349">
         <v>3608</v>
       </c>
-      <c r="B349">
-        <v>11.11</v>
+      <c r="B349" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C349">
         <v>100</v>
@@ -5299,8 +5308,8 @@
       <c r="A350">
         <v>3609</v>
       </c>
-      <c r="B350">
-        <v>11.11</v>
+      <c r="B350" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C350">
         <v>100</v>
@@ -5313,8 +5322,8 @@
       <c r="A351">
         <v>3610</v>
       </c>
-      <c r="B351">
-        <v>11.11</v>
+      <c r="B351" s="4">
+        <v>44181.548611111109</v>
       </c>
       <c r="C351">
         <v>100</v>
@@ -5327,22 +5336,22 @@
       <c r="A352">
         <v>3611</v>
       </c>
-      <c r="B352">
-        <v>11.11</v>
+      <c r="B352" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C352">
         <v>100</v>
       </c>
       <c r="D352" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A353">
         <v>3612</v>
       </c>
-      <c r="B353">
-        <v>11.11</v>
+      <c r="B353" s="1">
+        <v>44182.625</v>
       </c>
       <c r="C353">
         <v>100</v>
@@ -5355,8 +5364,8 @@
       <c r="A354">
         <v>3613</v>
       </c>
-      <c r="B354">
-        <v>11.11</v>
+      <c r="B354" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C354">
         <v>100</v>
@@ -5369,8 +5378,8 @@
       <c r="A355">
         <v>3614</v>
       </c>
-      <c r="B355">
-        <v>11.11</v>
+      <c r="B355" s="1">
+        <v>44182.5</v>
       </c>
       <c r="C355">
         <v>100</v>
@@ -5383,8 +5392,8 @@
       <c r="A356">
         <v>3615</v>
       </c>
-      <c r="B356">
-        <v>11.11</v>
+      <c r="B356" s="5">
+        <v>44182.708333333336</v>
       </c>
       <c r="C356">
         <v>100</v>
@@ -5397,8 +5406,8 @@
       <c r="A357">
         <v>3616</v>
       </c>
-      <c r="B357">
-        <v>11.11</v>
+      <c r="B357" s="1">
+        <v>44182.375</v>
       </c>
       <c r="C357">
         <v>100</v>
@@ -5411,8 +5420,8 @@
       <c r="A358">
         <v>3617</v>
       </c>
-      <c r="B358">
-        <v>11.11</v>
+      <c r="B358" s="1">
+        <v>44182.666666666664</v>
       </c>
       <c r="C358">
         <v>100</v>
@@ -5422,44 +5431,44 @@
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A359">
+      <c r="A359" s="2">
         <v>3618</v>
       </c>
-      <c r="B359">
-        <v>11.11</v>
-      </c>
-      <c r="C359">
+      <c r="B359" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C359" s="2">
         <v>-1</v>
       </c>
-      <c r="D359" t="s">
+      <c r="D359" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A360">
+      <c r="A360" s="2">
         <v>3619</v>
       </c>
-      <c r="B360">
-        <v>11.11</v>
-      </c>
-      <c r="C360">
+      <c r="B360" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C360" s="2">
         <v>-1</v>
       </c>
-      <c r="D360" t="s">
+      <c r="D360" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A361">
+      <c r="A361" s="2">
         <v>3620</v>
       </c>
-      <c r="B361">
-        <v>11.11</v>
-      </c>
-      <c r="C361">
+      <c r="B361" s="3">
+        <v>44182.375</v>
+      </c>
+      <c r="C361" s="2">
         <v>-1</v>
       </c>
-      <c r="D361" t="s">
+      <c r="D361" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
not perfect mypc finish
</commit_message>
<xml_diff>
--- a/data/mypc_dummy.xlsx
+++ b/data/mypc_dummy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="15">
   <si>
     <t>hakbun</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,46 @@
   </si>
   <si>
     <t>empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한컴 업데이트 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패스워드 까먹음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password 까먹음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAC 노트북 사용 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맥 노트북 때문에</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>패스워드 기억안남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한컴 NEO임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 까먹음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 기억 안남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비번 까먹음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -408,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -538,10 +578,10 @@
         <v>44182.5</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -776,10 +816,10 @@
         <v>44182.625</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
@@ -972,10 +1012,10 @@
         <v>44182.625</v>
       </c>
       <c r="C40">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
@@ -1350,10 +1390,10 @@
         <v>44182.625</v>
       </c>
       <c r="C67">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.4">
@@ -1532,10 +1572,10 @@
         <v>44182.5</v>
       </c>
       <c r="C80">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D80" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.4">
@@ -1658,10 +1698,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C89">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D89" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.4">
@@ -1742,10 +1782,10 @@
         <v>44183.375</v>
       </c>
       <c r="C95">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D95" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.4">
@@ -1784,10 +1824,10 @@
         <v>44182.5</v>
       </c>
       <c r="C98">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D98" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.4">
@@ -1966,10 +2006,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C111">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D111" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.4">
@@ -1980,10 +2020,10 @@
         <v>44182.375</v>
       </c>
       <c r="C112">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D112" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.4">
@@ -2078,10 +2118,10 @@
         <v>44181.548611111109</v>
       </c>
       <c r="C119">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D119" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.4">
@@ -2302,10 +2342,10 @@
         <v>44182.375</v>
       </c>
       <c r="C135">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D135" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.4">
@@ -2568,10 +2608,10 @@
         <v>44183.375</v>
       </c>
       <c r="C154">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D154" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.4">
@@ -2582,10 +2622,10 @@
         <v>44182.5</v>
       </c>
       <c r="C155">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D155" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.4">
@@ -2890,10 +2930,10 @@
         <v>44182.708333333336</v>
       </c>
       <c r="C177">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D177" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.4">
@@ -3002,10 +3042,10 @@
         <v>44182.708333333336</v>
       </c>
       <c r="C185">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D185" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.4">
@@ -3086,10 +3126,10 @@
         <v>44182.375</v>
       </c>
       <c r="C191">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D191" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.4">
@@ -3100,10 +3140,10 @@
         <v>44183.375</v>
       </c>
       <c r="C192">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D192" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.4">
@@ -3170,10 +3210,10 @@
         <v>44182.5</v>
       </c>
       <c r="C197">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D197" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.4">
@@ -3310,10 +3350,10 @@
         <v>44182.375</v>
       </c>
       <c r="C207">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D207" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.4">
@@ -3324,10 +3364,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C208">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D208" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.4">
@@ -3436,10 +3476,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C216">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D216" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.4">
@@ -3576,10 +3616,10 @@
         <v>44182.5</v>
       </c>
       <c r="C226">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D226" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.4">
@@ -3660,10 +3700,10 @@
         <v>44182.5</v>
       </c>
       <c r="C232">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D232" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.4">
@@ -3954,10 +3994,10 @@
         <v>44182.5</v>
       </c>
       <c r="C253">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D253" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.4">
@@ -4164,10 +4204,10 @@
         <v>44182.5</v>
       </c>
       <c r="C268">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D268" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.4">
@@ -4290,10 +4330,10 @@
         <v>44182.5</v>
       </c>
       <c r="C277">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D277" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.4">
@@ -4416,10 +4456,10 @@
         <v>44182.5</v>
       </c>
       <c r="C286">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D286" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.4">
@@ -4584,10 +4624,10 @@
         <v>44182.375</v>
       </c>
       <c r="C298">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D298" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.4">
@@ -4766,10 +4806,10 @@
         <v>44182.625</v>
       </c>
       <c r="C311">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D311" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.4">
@@ -4948,10 +4988,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C324">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D324" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.4">
@@ -4962,10 +5002,10 @@
         <v>44182.375</v>
       </c>
       <c r="C325">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D325" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.4">
@@ -5130,10 +5170,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C337">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D337" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.4">
@@ -5298,10 +5338,10 @@
         <v>44182.375</v>
       </c>
       <c r="C349">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D349" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.4">
@@ -5424,10 +5464,10 @@
         <v>44182.666666666664</v>
       </c>
       <c r="C358">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D358" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
mypc dummy xlsx modify
</commit_message>
<xml_diff>
--- a/data/mypc_dummy.xlsx
+++ b/data/mypc_dummy.xlsx
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H153" sqref="H153"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>